<commit_message>
fixed: put monsters on level 2 and playtested, fixed colors in stats bar, tweaked player starting stats, tweaked experience & gold from chests
</commit_message>
<xml_diff>
--- a/docs/NorthPolePatrol-Maps.xlsx
+++ b/docs/NorthPolePatrol-Maps.xlsx
@@ -245,9 +245,6 @@
     <t>3 goblins</t>
   </si>
   <si>
-    <t>2 blobs</t>
-  </si>
-  <si>
     <t>TRAIN3/stairs</t>
   </si>
   <si>
@@ -264,6 +261,9 @@
   </si>
   <si>
     <t>2 frost giants</t>
+  </si>
+  <si>
+    <t>1 blobs</t>
   </si>
 </sst>
 </file>
@@ -597,7 +597,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -896,6 +896,24 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -904,9 +922,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFE81CBC"/>
       <color rgb="FFFF9900"/>
       <color rgb="FF926A9A"/>
-      <color rgb="FFE81CBC"/>
       <color rgb="FF33CCCC"/>
       <color rgb="FFA5A5A5"/>
       <color rgb="FF9966FF"/>
@@ -3585,8 +3603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="V19" sqref="V19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4709,7 +4727,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A14" s="59">
         <v>5</v>
       </c>
@@ -4728,7 +4746,7 @@
       <c r="F14" s="83">
         <v>0</v>
       </c>
-      <c r="G14" s="97">
+      <c r="G14" s="10">
         <v>0</v>
       </c>
       <c r="H14" s="80">
@@ -4795,7 +4813,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:28" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="59">
         <v>5</v>
       </c>
@@ -5002,7 +5020,7 @@
         <v>69</v>
       </c>
       <c r="V18" s="82" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="W18" s="33"/>
       <c r="X18" s="17" t="s">
@@ -6871,7 +6889,7 @@
   <dimension ref="A1:AB38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U14" sqref="U14"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6962,14 +6980,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>0</v>
       </c>
       <c r="B2" s="3">
         <v>0</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="24">
         <v>0</v>
       </c>
       <c r="D2" s="3">
@@ -7026,7 +7044,7 @@
       <c r="U2" s="59">
         <v>5</v>
       </c>
-      <c r="V2" s="58">
+      <c r="V2" s="103">
         <v>5</v>
       </c>
       <c r="W2" s="59">
@@ -7048,17 +7066,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>0</v>
       </c>
-      <c r="B3" s="3">
-        <v>0</v>
-      </c>
-      <c r="C3" s="3">
-        <v>0</v>
-      </c>
-      <c r="D3" s="3">
+      <c r="B3" s="12">
+        <v>0</v>
+      </c>
+      <c r="C3" s="107">
+        <v>0</v>
+      </c>
+      <c r="D3" s="23">
         <v>0</v>
       </c>
       <c r="E3" s="58">
@@ -7109,13 +7127,13 @@
       <c r="T3" s="16">
         <v>16</v>
       </c>
-      <c r="U3" s="10">
-        <v>0</v>
-      </c>
-      <c r="V3" s="10">
-        <v>0</v>
-      </c>
-      <c r="W3" s="10">
+      <c r="U3" s="83">
+        <v>0</v>
+      </c>
+      <c r="V3" s="86">
+        <v>0</v>
+      </c>
+      <c r="W3" s="80">
         <v>0</v>
       </c>
       <c r="X3" s="10">
@@ -7134,14 +7152,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="99">
         <v>32</v>
       </c>
       <c r="B4" s="3">
         <v>0</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="31">
         <v>0</v>
       </c>
       <c r="D4" s="61">
@@ -7198,7 +7216,7 @@
       <c r="U4" s="10">
         <v>0</v>
       </c>
-      <c r="V4" s="10">
+      <c r="V4" s="87">
         <v>0</v>
       </c>
       <c r="W4" s="10">
@@ -7392,7 +7410,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="58">
         <v>5</v>
       </c>
@@ -7429,7 +7447,7 @@
       <c r="L7" s="58">
         <v>5</v>
       </c>
-      <c r="M7" s="3">
+      <c r="M7" s="24">
         <v>0</v>
       </c>
       <c r="N7" s="58">
@@ -7478,7 +7496,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="77">
         <v>13</v>
       </c>
@@ -7512,13 +7530,13 @@
       <c r="K8" s="58">
         <v>5</v>
       </c>
-      <c r="L8" s="58">
-        <v>5</v>
-      </c>
-      <c r="M8" s="3">
-        <v>0</v>
-      </c>
-      <c r="N8" s="58">
+      <c r="L8" s="104">
+        <v>5</v>
+      </c>
+      <c r="M8" s="106">
+        <v>0</v>
+      </c>
+      <c r="N8" s="105">
         <v>5</v>
       </c>
       <c r="O8" s="58">
@@ -7564,14 +7582,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>0</v>
       </c>
       <c r="B9" s="3">
         <v>0</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="24">
         <v>0</v>
       </c>
       <c r="D9" s="58">
@@ -7601,7 +7619,7 @@
       <c r="L9" s="5">
         <v>65</v>
       </c>
-      <c r="M9" s="3">
+      <c r="M9" s="31">
         <v>0</v>
       </c>
       <c r="N9" s="3">
@@ -7650,17 +7668,17 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="99">
         <v>58</v>
       </c>
-      <c r="B10" s="3">
-        <v>0</v>
-      </c>
-      <c r="C10" s="3">
-        <v>0</v>
-      </c>
-      <c r="D10" s="58">
+      <c r="B10" s="12">
+        <v>0</v>
+      </c>
+      <c r="C10" s="107">
+        <v>0</v>
+      </c>
+      <c r="D10" s="105">
         <v>5</v>
       </c>
       <c r="E10" s="63">
@@ -7736,14 +7754,14 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="58">
         <v>5</v>
       </c>
       <c r="B11" s="3">
         <v>0</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="31">
         <v>0</v>
       </c>
       <c r="D11" s="58">
@@ -7776,7 +7794,7 @@
       <c r="M11" s="3">
         <v>0</v>
       </c>
-      <c r="N11" s="3">
+      <c r="N11" s="24">
         <v>0</v>
       </c>
       <c r="O11" s="3">
@@ -7822,7 +7840,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="58">
         <v>5</v>
       </c>
@@ -7859,13 +7877,13 @@
       <c r="L12" s="61">
         <v>4</v>
       </c>
-      <c r="M12" s="3">
-        <v>0</v>
-      </c>
-      <c r="N12" s="3">
-        <v>0</v>
-      </c>
-      <c r="O12" s="3">
+      <c r="M12" s="12">
+        <v>0</v>
+      </c>
+      <c r="N12" s="30">
+        <v>0</v>
+      </c>
+      <c r="O12" s="23">
         <v>0</v>
       </c>
       <c r="P12" s="3">
@@ -7908,7 +7926,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="58">
         <v>5</v>
       </c>
@@ -7927,7 +7945,7 @@
       <c r="F13" s="3">
         <v>0</v>
       </c>
-      <c r="G13" s="3">
+      <c r="G13" s="24">
         <v>0</v>
       </c>
       <c r="H13" s="3">
@@ -7948,7 +7966,7 @@
       <c r="M13" s="3">
         <v>0</v>
       </c>
-      <c r="N13" s="3">
+      <c r="N13" s="31">
         <v>0</v>
       </c>
       <c r="O13" s="3">
@@ -7975,7 +7993,7 @@
       <c r="V13" s="10">
         <v>0</v>
       </c>
-      <c r="W13" s="69">
+      <c r="W13" s="102">
         <v>65</v>
       </c>
       <c r="X13" s="59">
@@ -7994,7 +8012,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="58">
         <v>5</v>
       </c>
@@ -8010,13 +8028,13 @@
       <c r="E14" s="3">
         <v>0</v>
       </c>
-      <c r="F14" s="3">
-        <v>0</v>
-      </c>
-      <c r="G14" s="3">
-        <v>0</v>
-      </c>
-      <c r="H14" s="3">
+      <c r="F14" s="12">
+        <v>0</v>
+      </c>
+      <c r="G14" s="30">
+        <v>0</v>
+      </c>
+      <c r="H14" s="23">
         <v>0</v>
       </c>
       <c r="I14" s="58">
@@ -8058,13 +8076,13 @@
       <c r="U14" s="10">
         <v>0</v>
       </c>
-      <c r="V14" s="10">
-        <v>0</v>
-      </c>
-      <c r="W14" s="10">
-        <v>0</v>
-      </c>
-      <c r="X14" s="10">
+      <c r="V14" s="83">
+        <v>0</v>
+      </c>
+      <c r="W14" s="86">
+        <v>0</v>
+      </c>
+      <c r="X14" s="80">
         <v>0</v>
       </c>
       <c r="Y14" s="10">
@@ -8080,7 +8098,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A15" s="58">
         <v>5</v>
       </c>
@@ -8099,7 +8117,7 @@
       <c r="F15" s="58">
         <v>5</v>
       </c>
-      <c r="G15" s="3">
+      <c r="G15" s="31">
         <v>0</v>
       </c>
       <c r="H15" s="3">
@@ -8147,7 +8165,7 @@
       <c r="V15" s="10">
         <v>0</v>
       </c>
-      <c r="W15" s="10">
+      <c r="W15" s="87">
         <v>0</v>
       </c>
       <c r="X15" s="10">
@@ -8281,13 +8299,13 @@
     </row>
     <row r="18" spans="1:25" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="R18" s="40" t="s">
+        <v>73</v>
+      </c>
+      <c r="T18" s="79" t="s">
         <v>74</v>
       </c>
-      <c r="T18" s="79" t="s">
+      <c r="V18" s="82" t="s">
         <v>75</v>
-      </c>
-      <c r="V18" s="82" t="s">
-        <v>76</v>
       </c>
       <c r="W18" s="33"/>
       <c r="X18" s="17" t="s">
@@ -8322,7 +8340,7 @@
         <v>8</v>
       </c>
       <c r="C20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F20" s="70">
         <v>28</v>
@@ -8345,7 +8363,7 @@
         <v>7</v>
       </c>
       <c r="C21" s="49" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F21" s="70">
         <v>29</v>
@@ -8571,7 +8589,7 @@
         <v>40</v>
       </c>
       <c r="G32" s="71" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K32" s="47">
         <v>60</v>

</xml_diff>

<commit_message>
fixed: added monsters to level 3 & playtested. Updated win and death messaging.
</commit_message>
<xml_diff>
--- a/docs/NorthPolePatrol-Maps.xlsx
+++ b/docs/NorthPolePatrol-Maps.xlsx
@@ -440,7 +440,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -601,11 +601,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF33CCCC"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF33CCCC"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF33CCCC"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF33CCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -922,6 +937,21 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -930,10 +960,10 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF33CCCC"/>
       <color rgb="FFE81CBC"/>
       <color rgb="FFFF9900"/>
       <color rgb="FF926A9A"/>
-      <color rgb="FF33CCCC"/>
       <color rgb="FFA5A5A5"/>
       <color rgb="FF9966FF"/>
       <color rgb="FFFF6600"/>
@@ -8743,7 +8773,7 @@
   <dimension ref="A1:AB38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="U1" sqref="U1:U13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8834,7 +8864,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>0</v>
       </c>
@@ -8901,7 +8931,7 @@
       <c r="V2" s="102">
         <v>5</v>
       </c>
-      <c r="W2" s="58">
+      <c r="W2" s="111">
         <v>5</v>
       </c>
       <c r="X2" s="10">
@@ -8920,7 +8950,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>0</v>
       </c>
@@ -8957,7 +8987,7 @@
       <c r="L3" s="3">
         <v>0</v>
       </c>
-      <c r="M3" s="3">
+      <c r="M3" s="24">
         <v>0</v>
       </c>
       <c r="N3" s="3">
@@ -8984,13 +9014,13 @@
       <c r="U3" s="82">
         <v>0</v>
       </c>
-      <c r="V3" s="3">
-        <v>0</v>
-      </c>
-      <c r="W3" s="79">
-        <v>0</v>
-      </c>
-      <c r="X3" s="10">
+      <c r="V3" s="12">
+        <v>0</v>
+      </c>
+      <c r="W3" s="112">
+        <v>0</v>
+      </c>
+      <c r="X3" s="79">
         <v>0</v>
       </c>
       <c r="Y3" s="58">
@@ -9006,7 +9036,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>61</v>
       </c>
@@ -9040,13 +9070,13 @@
       <c r="K4" s="3">
         <v>0</v>
       </c>
-      <c r="L4" s="3">
-        <v>0</v>
-      </c>
-      <c r="M4" s="3">
-        <v>0</v>
-      </c>
-      <c r="N4" s="3">
+      <c r="L4" s="12">
+        <v>0</v>
+      </c>
+      <c r="M4" s="110">
+        <v>0</v>
+      </c>
+      <c r="N4" s="23">
         <v>0</v>
       </c>
       <c r="O4" s="3">
@@ -9073,7 +9103,7 @@
       <c r="V4" s="86">
         <v>0</v>
       </c>
-      <c r="W4" s="10">
+      <c r="W4" s="86">
         <v>0</v>
       </c>
       <c r="X4" s="10">
@@ -9092,7 +9122,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A5" s="57">
         <v>5</v>
       </c>
@@ -9129,7 +9159,7 @@
       <c r="L5" s="3">
         <v>0</v>
       </c>
-      <c r="M5" s="3">
+      <c r="M5" s="31">
         <v>0</v>
       </c>
       <c r="N5" s="69">
@@ -9264,7 +9294,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="57">
         <v>5</v>
       </c>
@@ -9337,7 +9367,7 @@
       <c r="X7" s="10">
         <v>0</v>
       </c>
-      <c r="Y7" s="10">
+      <c r="Y7" s="83">
         <v>0</v>
       </c>
       <c r="Z7" s="10">
@@ -9350,7 +9380,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>0</v>
       </c>
@@ -9369,7 +9399,7 @@
       <c r="F8" s="62">
         <v>46</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="24">
         <v>0</v>
       </c>
       <c r="H8" s="3">
@@ -9411,7 +9441,7 @@
       <c r="T8" s="60">
         <v>4</v>
       </c>
-      <c r="U8" s="10">
+      <c r="U8" s="83">
         <v>0</v>
       </c>
       <c r="V8" s="10">
@@ -9420,13 +9450,13 @@
       <c r="W8" s="10">
         <v>0</v>
       </c>
-      <c r="X8" s="10">
-        <v>0</v>
-      </c>
-      <c r="Y8" s="10">
-        <v>0</v>
-      </c>
-      <c r="Z8" s="10">
+      <c r="X8" s="82">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="112">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="79">
         <v>0</v>
       </c>
       <c r="AA8" s="76">
@@ -9436,7 +9466,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>0</v>
       </c>
@@ -9452,13 +9482,13 @@
       <c r="E9" s="57">
         <v>5</v>
       </c>
-      <c r="F9" s="57">
-        <v>5</v>
-      </c>
-      <c r="G9" s="3">
-        <v>0</v>
-      </c>
-      <c r="H9" s="3">
+      <c r="F9" s="103">
+        <v>5</v>
+      </c>
+      <c r="G9" s="30">
+        <v>0</v>
+      </c>
+      <c r="H9" s="23">
         <v>0</v>
       </c>
       <c r="I9" s="57">
@@ -9494,13 +9524,13 @@
       <c r="S9" s="57">
         <v>5</v>
       </c>
-      <c r="T9" s="10">
-        <v>0</v>
-      </c>
-      <c r="U9" s="10">
-        <v>0</v>
-      </c>
-      <c r="V9" s="10">
+      <c r="T9" s="82">
+        <v>0</v>
+      </c>
+      <c r="U9" s="112">
+        <v>0</v>
+      </c>
+      <c r="V9" s="79">
         <v>0</v>
       </c>
       <c r="W9" s="58">
@@ -9509,7 +9539,7 @@
       <c r="X9" s="99">
         <v>17</v>
       </c>
-      <c r="Y9" s="10">
+      <c r="Y9" s="86">
         <v>0</v>
       </c>
       <c r="Z9" s="10">
@@ -9522,14 +9552,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="60">
         <v>4</v>
       </c>
-      <c r="B10" s="3">
-        <v>0</v>
-      </c>
-      <c r="C10" s="24">
+      <c r="B10" s="12">
+        <v>0</v>
+      </c>
+      <c r="C10" s="30">
         <v>0</v>
       </c>
       <c r="D10" s="104">
@@ -9541,7 +9571,7 @@
       <c r="F10" s="57">
         <v>5</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10" s="31">
         <v>0</v>
       </c>
       <c r="H10" s="3">
@@ -9583,7 +9613,7 @@
       <c r="T10" s="58">
         <v>5</v>
       </c>
-      <c r="U10" s="58">
+      <c r="U10" s="93">
         <v>5</v>
       </c>
       <c r="V10" s="58">
@@ -9608,7 +9638,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A11" s="57">
         <v>5</v>
       </c>
@@ -9694,7 +9724,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="57">
         <v>5</v>
       </c>
@@ -9728,7 +9758,7 @@
       <c r="K12" s="57">
         <v>5</v>
       </c>
-      <c r="L12" s="3">
+      <c r="L12" s="24">
         <v>0</v>
       </c>
       <c r="M12" s="12">
@@ -9780,7 +9810,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:28" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="57">
         <v>5</v>
       </c>
@@ -9811,13 +9841,13 @@
       <c r="J13" s="57">
         <v>5</v>
       </c>
-      <c r="K13" s="57">
-        <v>5</v>
-      </c>
-      <c r="L13" s="3">
-        <v>0</v>
-      </c>
-      <c r="M13" s="3">
+      <c r="K13" s="103">
+        <v>5</v>
+      </c>
+      <c r="L13" s="110">
+        <v>0</v>
+      </c>
+      <c r="M13" s="23">
         <v>0</v>
       </c>
       <c r="N13" s="31">
@@ -9866,7 +9896,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A14" s="57">
         <v>5</v>
       </c>
@@ -9885,7 +9915,7 @@
       <c r="F14" s="12">
         <v>0</v>
       </c>
-      <c r="G14" s="30">
+      <c r="G14" s="3">
         <v>0</v>
       </c>
       <c r="H14" s="23">
@@ -9900,7 +9930,7 @@
       <c r="K14" s="57">
         <v>5</v>
       </c>
-      <c r="L14" s="5">
+      <c r="L14" s="109">
         <v>61</v>
       </c>
       <c r="M14" s="3">
@@ -9952,7 +9982,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:28" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="57">
         <v>5</v>
       </c>
@@ -10155,7 +10185,7 @@
       <c r="R18" s="81" t="s">
         <v>75</v>
       </c>
-      <c r="T18" s="78" t="s">
+      <c r="T18" s="108" t="s">
         <v>77</v>
       </c>
       <c r="V18" s="107" t="s">

</xml_diff>